<commit_message>
Get daily reddit data: Tue Feb 20 08:07:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_25.xlsx
+++ b/data/2024_02_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C448"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2505 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1avc2u5</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Vegas nails 💰</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qyr2ejj2pjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1avbnug</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Does anyone else find doing these soooo relaxing?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avbnug</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1avbd58</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>🌚</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4itgv6juojc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1av9pff</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Seeking advice on One Kill Gel Remover and Peel off base gel.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av9pff/seeking_advice_on_one_kill_gel_remover_and_peel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1av9xym</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Summer flowers</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av9xym</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1av9wdt</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Brown Frenchies</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av9wdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1av9nor</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Can these be easily fixed, and do they need to be?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av9nor/can_these_be_easily_fixed_and_do_they_need_to_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1av9aod</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Really love the circle on the thumb 💙</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oojqlo439ojc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1av8ymb</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>How long should you wait between gelx sets?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av8ymb/how_long_should_you_wait_between_gelx_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1av6amc</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>what I got (@nailsbysandyyy) vs the inspiration (@slayedbysarena)</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av6amc</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1av5oka</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Good LED lights for curing??</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av5oka/good_led_lights_for_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1av5m8d</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>I’m looking for a gold nail art pen that I saw on instagram. Does anyone know what I’m talking about?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av5m8d/im_looking_for_a_gold_nail_art_pen_that_i_saw_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1av8rk1</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Solid Gel Glue for Apres Neutral tips?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av8rk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1av8jtt</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Press on opinions💅</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4xqifgu1ojc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1av79qz</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Nails were looking heinous so i decided to put my acrylics back on!</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av79qz</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1av6sn0</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Belated valentines nails</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5043gpt7mnjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1av6mlw</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Russian manicure</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av6mlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1av6m3p</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Can't go wrong</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8lclsuoknjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1av6icn</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>A husband on a mission - this little piggy went to market, this little piggy is a little abstract?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pn6nf01tjnjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1av6eto</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>under the sea but not really 🐟</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av6eto</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1av6egm</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm loving this color scheme 😍 </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zawrispwinjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1av6aqh</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Beginner nail tech</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av6aqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1av5ryk</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>how to save my nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av5ryk</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1av5qw0</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Playing with Foil</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an904c9ndnjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1av599v</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Little late but my valentines nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av599v</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1av50kk</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>glueing press ons</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av50kk/glueing_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1av3wqu</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>🎀🤍✨</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffqwofllymjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1av3b9e</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Gel x is so annoying</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av3b9e/gel_x_is_so_annoying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1av4osr</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Help with press ons - cuticle issue</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av4osr/help_with_press_ons_cuticle_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1av4iy3</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>First time doing soft gel tips on another person</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av4iy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1av4hmc</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>New Pink &amp; Black Manicure 🩷🖤 {Matte}</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bev024d93njc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1av48ih</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Are "Cat Eyes" still cute?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozzdc8x71njc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1av3q22</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>jewel kitty nails~ ♡</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av3q22</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1av3hno</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Collection of my favorite nails</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av3hno</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1av3dcb</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>dnd liquid chrome</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av3dcb/dnd_liquid_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1av2z8j</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Magnet Magic</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y69fsjmermjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1av2hre</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>I'm officially a reformed nail-biter after 25 years! I celebrated with my first manicure on natural nails. Scroll over for naked-nail pic.</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av2hre</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1av2dt0</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Pain / tenderness after gel x removal</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1av2dt0/pain_tenderness_after_gel_x_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1av20lq</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Opinions needed</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av20lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1av1zyb</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just learned how to encapsulate! </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kg8wyagfkmjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1av1qxn</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>My super late valentine nails lol</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpqftlnmimjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1auzx2z</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Almost spring :)</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2ye6uhx5mjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1auzmea</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Press on nail glue question</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq0tbzyu3mjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1auz93r</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Conversation hearts 🥰They’re a little grown out and it’s past Valentine’s Day but I still wanted to share!</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umk8ipi81mjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1auz5uf</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>advice</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1auz5uf/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1auyngy</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>I need ideas for my new set please !</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dfe3cd3xljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1auyg6o</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Prob shouldn't paint my nails at night without glasses but I'm glad my natural nails are growing again</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auyg6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1auxzty</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>I haven’t been this WOWED by a polish combo in a very long while😵‍💫 Clickbait by Color Club topped with Now &amp; Zen by KBShimmer😍</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0il7jjnsljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1auxyj5</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>First time trying mirror chrome …</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auxyj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1auxmrz</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Love organising my polish :)</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1auxmrz/love_organising_my_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1auxkyn</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>How bad is it?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yw6q62gspljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1auwpo7</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>First time trying false nails! Opinions? :)</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auwpo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1auwitn</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Newest set ❤️ working on growing my nails out!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zza0nhymiljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1auw1d9</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Chipping/peeling</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1auw1d9/chippingpeeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1auva9w</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>my sets since I’ve been able to do my nails again, what do you think?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auva9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1auv76t</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Icy and sparkly nails ❄️</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqq9ussh9ljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1auv549</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>DIY black jelly nails with some flowers 🖤🌼</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt859gp39ljc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1auulhe</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Back to basics 🌸</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ip7ds8d5ljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1auujsq</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Birthday nails for my 21st</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auujsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1auuaia</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>In need of some advice with gel polish lifting on natural nails. I feel like I've exhausted everything and can not seem to find a solution that will extend my gel polish beyond 2-3 days before they start lifting.</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1auuaia/in_need_of_some_advice_with_gel_polish_lifting_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1auu1m1</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>What's a good top coat??</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1auu1m1/whats_a_good_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1autzsw</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Clown nails🤹🤡</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fkver681ljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1aut993</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>80s nails :)</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aut993</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1aus45l</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>The month of love</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aus45l</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1aut5i7</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Did you guys charge hen you where first starting out?!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aut5i7/did_you_guys_charge_hen_you_where_first_starting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1aut514</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Clear French tips</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4237nzlevkjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1au6k7r</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>How can I make my nails cleaner looking??</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1au6k7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ausy2y</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>LCN nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ausy2y/lcn_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1aus1b6</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>First time using builder gel &amp; doing designs. What do you think?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aus1b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1aurq93</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I need help learning to take care for my nails!!</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aurq93</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1aurobd</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>New set 🐊🤍</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4dejp7alkjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1auqiaz</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>My nails grow out too fast!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxgfyz55dkjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1aup2u5</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Im so sad 😞</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv1mtazb2kjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1aun8l6</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>It’s been a year since I kicked a 25 year long nail biting habit, and I’m finally starting to see nail bed growth/reattachment!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j294yye6njjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1aun7nt</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Matchy Monday</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aun7nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1aumvli</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Best paper to use for polish swatches?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aumvli/best_paper_to_use_for_polish_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1aum8d8</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Especially loved this color and design</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqb61ogqdjjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1aul2iw</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Mid February nail sets that I've made</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aul2iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1auk5l7</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>I love marble nails!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auk5l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1aubd70</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>A crossover of my two faves (r/bathandbodyworks and r/nails)</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcjmji8b6gjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1augjzn</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Got gel nail extensions, wanted shellac polish on my real nail instead. Will they ever come off?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1augjzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1avc87s</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Very white tips on the free edge + jelly polish?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avc87s/very_white_tips_on_the_free_edge_jelly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1avc7lk</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Top coat that darkens, like Sally Hansen Big Smoky Top Coat?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avc7lk/top_coat_that_darkens_like_sally_hansen_big_smoky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1avbxxm</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Glitter smoothing top coat and drying time</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avbxxm/glitter_smoothing_top_coat_and_drying_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1av6ccg</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Blue Skittle</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av6ccg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1av511j</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Now Thrive</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av511j</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1av4uwz</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Fake halo is sick 🤩</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av4uwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1av4pf9</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Ze Vampir</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av4pf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1av4d9i</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Is there a way to get nails like this with regular polish? I think these photos are gel but I could be wrong. Any recs?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av4d9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1av482w</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Time for a Change?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av482w</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1av3tnj</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>My partner called these “pesto nails” 🫠</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9c15eixxmjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1av3sgs</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Reminds me of a mood ring</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7gnfzq5fxmjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1av3gki</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chlorine and nail polish? </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1av3gki/chlorine_and_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1av3ay6</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>I Can Buy Myself Flowers ✨️</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av3ay6</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1av2ei1</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>This is the same polish with and without flash 💜💙</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfghpbzbnmjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1av1qq3</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Twilight Tanzanite</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av1qq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1av0kzf</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Lunar New Year skittle 🐉✨</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av0kzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1av0cxs</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Need Help Identifying A Polish</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htkmxaww8mjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1av00bg</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Skittles</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz7i3egk6mjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1auzznz</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Beaux Rêves Lacquer - Blooming Azalea</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auzznz</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1auzjm9</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Space Themed Nails</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auzjm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1auz0s8</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>indigo/blue polishes that are similar?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/loaxrn9nzljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1auyxv3</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>newbie help</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1auyxv3/newbie_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1auy97r</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Velvet nails using Mani Mags</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0swn3yrduljc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1auy22s</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>My valentines date nails</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auy22s</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1auxylh</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>I haven’t been this WOWED by a polish combo in a very long while😵‍💫 Clickbait by Color Club topped with Now &amp; Zen by KBShimmer😍</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iaqeerfsljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1auxckj</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Le Mini Macaron - Café Crème</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx515p37oljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1aux63i</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>CHANEL 531 Peridot</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aux63i</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1auwyv8</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Zoya Twila over OPI Russian Navy</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bagojvmlljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1auw1vo</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>LynB and Dany Vianna Combo</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v67udhxefljc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1auvmm0</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Duo of Lilac 💜</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/apsvmch</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1auv2pi</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>The Little Prince</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auv2pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1auv1xn</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Flakies and stickers</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auv1xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1auss9d</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Holo Taco Crimson Void</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auss9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1autw2i</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Trouvaille has my heart ❤️</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1autw2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1autu8b</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>OPI Red Hot Rio</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1autu8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1au6fg9</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Out of the blue</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em8bjc9m3fjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1autgc9</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Getting into stamping</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1autgc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1autcw7</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Dots, dashes and tiny stars</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfgrrlhxwkjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1aut8oc</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Gel polish shower woes</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aut8oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1aust4l</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Goblins and Ghoulies 🤤</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/geylbjb3tkjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ausdan</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>SNS v Gelx v Acrylic</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ausdan/sns_v_gelx_v_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1aus211</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>More Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aus211</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1aurxzp</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>First Thermal on a cold day</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aurxzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1auroyk</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Poison Garden by Envy Lacquer! featuring South Lake Tahoe snow✨✨✨</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auroyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1aurnn7</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Can anyone speak to the opacity of this shade/formula? [PPU Strange the Dreamer by Atomic Polish]</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aurnn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1aurjxk</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Electric - a perfect word for this polish</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aurjxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1auqvah</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Yellow to Purple skittle</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvlfnfbnfkjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1auqtbl</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>was not expecting it to be so damn glowy 🫢</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auqtbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1auq5gd</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Millennia in the sun ☀️</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auq5gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1auns2e</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>When your favorite neon purple turns pink 😢</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecai2bztrjjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1aun4fr</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Clionadh — Lux</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aun4fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1aumgqi</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Mannequin nails recommendations</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aumgqi/mannequin_nails_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1aukpqz</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aukpqz/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1auj6v7</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Acetone Antidote to a pot/sponge remover?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auj6v7</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1avagra</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Claude Monet inspired set</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtvaxqzrkojc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1av8epr</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>MINECRAFT NAILS</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av8epr</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1av62ri</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>spring inspo</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jf1b2a9gnjc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1av3ql4</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>finally got around to making a set with these kitty decals~ ♡</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1av3ql4</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1av14fy</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Pinterest Inspired Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz1aaut9emjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1av0t3r</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>I tried something new while i had some free time. Can that be seen? First time hand painted 🙈</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq7xwhxybmjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1auzbrk</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Another set I cannot stop staring at!</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auzbrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1aupu93</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Kiddo wanted valentines nails</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhsl5vj68kjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1auptt9</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Pink nails, wishing the spring welcome 🌸</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1f6udy738kjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1aun4rx</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>late valentine nails for my bestie</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qj66lmg8mjjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1auk700</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>I love marble nails!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1auk700</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1aujpuq</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Did a whole set of polygel nails on myself. Paint job is not the best but I still liked it.</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0cbmrlxilijc1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb 21 08:08:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_25.xlsx
+++ b/data/2024_02_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C448"/>
+  <dimension ref="A1:C598"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8049,6 +8049,2556 @@
         </is>
       </c>
     </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1aw63tm</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>DIY mocha nails 💅</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw63tm</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1aw5wks</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Freshly filed! Still working on getting all the nails to the same shape. I'd love coffin but prefer shorter nails</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw5wks</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1avyoe5</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>It’s giving Crocodile. Or maybe even a Dragon.</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0osnqqlf8ujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1aw3tsg</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>2 week nail growth</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw3tsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1aw3am6</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Growing nails out for first time, why do they look like this?💀</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6bztufmbvjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1aw3aic</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Tech removed shellac with just a grinder??</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aw3aic/tech_removed_shellac_with_just_a_grinder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1aw303z</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Got engaged then did my nails lol</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/12qvouwz8vjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1aw2z3h</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Which shape?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4o4b89xp8vjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1aw2qhz</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Love!!</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ku13w5nj6vjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1aw2fsd</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>This set took me forever but here i am!! I’m so proud!! Vs my before is at the end!!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw2fsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1aw2d7a</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Best shape for my hands?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw2d7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1aw28jk</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>I am a painter &amp; a nail tech👩‍🎨</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw28jk</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1aw1uk9</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vp3vrupyujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1aw1obe</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>What shape are these?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21axskw7xujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1aw0wwe</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Friend did my nails for Awesome Con!</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmmtv9btqujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1aw0v2z</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>My after Valentines nails</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw0v2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1aw0uur</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Extra gel</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw0uur</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1aw0ufk</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Springtime nails ✨</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnw6qma9qujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1aw0pjc</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>What color nails do you recommend with nude heels and a bronze/copper dress?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aw0pjc/what_color_nails_do_you_recommend_with_nude_heels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1avz8vt</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Nail strengthener before applying gel polish</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avz8vt/nail_strengthener_before_applying_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1avyeek</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Most recent set for my client🌟💋</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avyeek</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1avy766</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>First time painting press-ons✨</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avy766</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1avy5ot</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Was going for a Mob Wives accent nail design. Should I make the nails all matte or just keep the accent nails glossy?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avy5ot</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1avy33l</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Gel acrylic is breaking and polish peeled off</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avy33l</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1avxolq</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haha has anyone done chickens? My wildest request yet. It even has double yolks. </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lty1u32s0ujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1avxbyb</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>What color should I paint them</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayajsko5ytjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1avwop6</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Side callouses.</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avwop6/side_callouses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1avw7b1</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Longer lasting alternative to led/uv glue </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avw7b1/longer_lasting_alternative_to_leduv_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1avw5a6</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>New Nails for my engagement!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avw5a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1avvvzn</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Curved nail</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10uvzr9lntjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1avvt0d</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Traveling and nails?!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic4hneuzmtjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1avvois</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day Set!!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kfszecv4mtjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1avvl2u</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>UV Pop Art Valentines Set</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avvl2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1avvj3e</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Which shape looks better on me?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avvj3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1avvf5e</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Pink Mermaid Vibes 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avvf5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1avv51z</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Officially a builder gel convert 🩵</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avv51z</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1avv50g</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>This design 😍</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sifk8r7itjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1avuqbz</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>What shape would u even classify these as</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqcp5cy9ftjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1avukwy</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Simple flower designs are my favorite 🌼</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1vtw6q8etjc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1avucto</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time since being a teenager.</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avucto</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1avtojj</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>What is it called for a clear coat mani and pedi?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avtojj</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1avtg5k</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>I love glitter on nails</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avtg5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1avszm8</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>My natural nails under hard gel look so bad - help!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avszm8/my_natural_nails_under_hard_gel_look_so_bad_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1avso4p</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>BDay Nails💕</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avso4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1avsmay</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Need ideas for my new nails! So stuck</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2shi6bpg0tjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1avqvx0</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Nude shorties</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxn9u1pcosjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1avqou5</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Do these look too far from the cuticle? 2-day old manicure</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igcak07xmsjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1avqpff</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Tweed nails for my younger sister</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avqpff</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1avqgpv</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Wanting to change up my shape/length. Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avqgpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1avqd04</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Love me a fun set of skittles 💅</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zax05ejlksjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1avq3gt</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>New Technician!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avq3gt</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1avpzah</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Red nails</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsw0224rhsjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1avpa9z</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>How long should it take for nail hardener to work?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avpa9z/how_long_should_it_take_for_nail_hardener_to_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1avp462</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Help - what kind of manicure is best for me?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avp462/help_what_kind_of_manicure_is_best_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1avoto1</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>When I Ignore everyone for the one ignoring me 🤡</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1z4tijl9sjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1avopgq</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I wish to know whether darker colours look better on my hand or lighter nudes? I'm thinking of getting light blue shade next time. Need help!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avopgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1avon90</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Vampy nails by me:D</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf6cttnd8sjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1avl9wv</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>new nails tomorrow, can’t decide on shape</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avl9wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1avjurx</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Can someone give me a step by step guide/tips/tricks/advice on how to remove hard gel at home?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avjurx/can_someone_give_me_a_step_by_step/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1avjdrf</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Acrylic nail is lifting. What do i do?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avjdrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1avfbiu</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>What glue do you use if your nails stay on for two weeks with normal use?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avfbiu/what_glue_do_you_use_if_your_nails_stay_on_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1avnm4s</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>My peachy nail design.</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avnm4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1avnlth</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Cute Spring Nails By @ xoyanie</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avnlth</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1avnkve</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Naturally long nails are starting to annoy me. Would a short coffin shape still give me a refined look?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avnkve</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1avni3a</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>My nail artist is literally a goddess</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4xe5xif0sjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1avn6il</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Finger tattoos distracting from nails</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avn6il/finger_tattoos_distracting_from_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1avmu9k</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Can’t beat a classic French</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mch2mfnvvrjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1avmkrt</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>I made myself some pink nails. Also I would love some suggestions for the next set :)</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbmbjdh1urjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1avm90t</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>what nail design/shape would look best for my hands?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11ehexoprrjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1avkrnj</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Lapis Lazuli Nails with Charm</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id0h28g6hrjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1avk82h</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Which shape best on me?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avk82h</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1avjt5w</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>I promised myself I'd get a subtle color 🥲 I'm so happy I didn't!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94y289k0arjc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1avhsu4</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Hearts of purple spring</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avhsu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1avh53l</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>I usually get the same shape (almond i think?) but was wondering what y’all think is the best shape for my hands? tia! 🩷</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avh53l</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1avg6id</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Your tips for protecting hands from lamp's UV light</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avg6id/your_tips_for_protecting_hands_from_lamps_uv_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1avfex0</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>For those who apply their own nails, what glue do you use and how? How long do your nails stay on with normal hand use?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avfex0/for_those_who_apply_their_own_nails_what_glue_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1avewqg</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Got my nails redone, just in time for spring</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avewqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1avesfv</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Measuring nails for press ons question</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1avesfv/measuring_nails_for_press_ons_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1aw3yp0</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>cat eye gel recs ??</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aw3yp0/cat_eye_gel_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1aw3n9d</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Mood: broken ankle</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgmyto40fvjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1aw2ogs</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Milka Mani!! Wisteria by Paradox Polish from Jan’s PPU</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw2ogs</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1aw2j8j</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque’s Encore Collection </t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0ozeajq4vjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1aw2hb2</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Let the swatching commence!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw2hb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1aw29tg</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Purple 💜</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw29tg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1aw24q8</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Cirque Colors “Bisou Bisou” issue?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztjo05e81vjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1aw1som</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Embrace the Mess was even better than expected!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iiv740x9yujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1aw1i0b</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Favorite colors, go!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aw1i0b/favorite_colors_go/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1aw12cw</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>The WAY Unicorn Pigment twinkles in the sun 🥵</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/esickq93sujc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1aw11qs</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Did my nails to match the weather—can you tell my hands are cold?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw11qs</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1aw0t8o</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Picked a red even after Valentines</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw0t8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1avyb0b</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>First ILNP polish, loving the sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avyb0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1avy4la</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forgot how good this color is </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4800f7n54ujc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1avxb3l</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Destashing top/base coats</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avxb3l/destashing_topbase_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1avwuyg</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Magnetic Nail art?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avwuyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1avwr4s</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Pink glitter!!</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avwr4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1avwggm</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>I managed to do the water marble technique!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avwggm</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1avv6vc</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>ILNP - Princeton is much more pleasant than expect4ed</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avv6vc/ilnp_princeton_is_much_more_pleasant_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1avv6iv</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Cuticles are always dry and peeling...I'm out of options</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avv6iv/cuticles_are_always_dry_and_peelingim_out_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1avuqnf</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Goodbye, Firefly Forest, hello....</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avuqnf/goodbye_firefly_forest_hello/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1avu0dr</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Gwyn</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avu0dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1avty2t</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>I need help!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avty2t/i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1avt1n0</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>My husband made me new displays for my swatch sticks!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avt1n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1avsdgy</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>My New Favorite Green 💚</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avsdgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1avs9j3</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Can someone give me a step by step guide/tips/tricks/advice on how to remove hard gel at home?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avs9j3/can_someone_give_me_a_step_by_step/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1avs5ec</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>ELI5 Nail Files?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avs5ec/eli5_nail_files/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1avro2a</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>A “flashy” sheer</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlcvej5wtsjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1avrhwi</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lacquerista Anniversary </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpard4hnssjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1avrcyd</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Sleeping on the perfect color for me?!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gktr0itorsjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1avr8x7</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>I’m still learning but how do these look? What could I have done differently?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mi00gk9tqsjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1avr3tp</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Twisted terracotta tanzanite</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avr3tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1avqefb</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>White or bridal crelly with flakies or glitter?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vaykmusvksjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1avplgd</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Jade nails</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avplgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1avpjil</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Essie Allure</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avpjil</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1avp2us</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>How to fix shrinkage once it happens?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avp2us/how_to_fix_shrinkage_once_it_happens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1avo6au</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Hello stunning multi-chrome!</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83xs9ez45sjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1avnw4c</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>What do you want in a polish??</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avnw4c/what_do_you_want_in_a_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1avmwal</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Lumen polishes are magical</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/usmtpkp8wrjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1avmtpl</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Fairy dust looks good over everything ✨</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avmtpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1avmqhv</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day Nails</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/BJFd3zh.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1avm7qv</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Aquariuuuuuuus! Aquaaaaaareeeeeuuuuussss!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avm7qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1avlryz</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Short gel x nails for long nail beds?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scb7uondorjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1avlpfw</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>I’m getting better and better at magnetic nails but I hate the time.</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/helortysnrjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1avew68</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Trying out shades from my Cirque haul! Polishes Used: Cirque Colors (Shade: Mosaic) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avew68</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1avkxa5</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>When your thermal is thermal-ing backwards</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aiu1klecirjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1avkrw9</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Swatched my whole collection</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avkrw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1avkodf</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Experience with Transform by Dazzle Dry?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avkodf/experience_with_transform_by_dazzle_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1avj7ag</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A springtime skittle </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9devc3c5rjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1avj36s</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Suuperr subtle jelly gradient</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avj36s</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1aviqaw</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>First Real At-Home Success!!</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c40jph8l1rjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1avhmeo</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Literal Skittles</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2q1dthdsqjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1avhez7</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Forbidden Cove by Mooncat</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/prjk6gxhqqjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1avg9l2</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are milk bath nails passé these days? </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srgqg77lfqjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1avfg3g</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>OPI top coat won't dry</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avfg3g/opi_top_coat_wont_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1aveyhb</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>I got jealous of your pretty sheer polishes so I layered my toppers</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujjmduef1qjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1avdjc3</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>press-ons with glitter dip powder</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avdjc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1aw2017</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Can you believe these are watercolor painting ?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw2017</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1aw1v11</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Vintage heart nails made by me</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aw1v11</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1avyqp5</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Last year I had to stop doing my own nails because I developed an allergy to UV gel. I missed it so much that a few weeks ago I started making nail sets just for fun! Here are my latest creations, that also are my first false nails sets.</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avyqp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1avwd2l</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>French Tips</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtmr5l62rtjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1avward</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Short square acrylic nails </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42kj8ogkqtjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1avvdmy</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Hand painted by me. Do you like my work?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwe0uwvwjtjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1avt88t</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Be brutally honest pls i want to learn!</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avt88t</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1avrp9i</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Just did my nails!💅🏼</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6f7e1zy3usjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1avrd4q</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>new nails🍒</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/00o5oe2qrsjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1avov1s</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>When I Ignore everyone for the one ignoring me 🤡</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75z5wtpv9sjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1avors2</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>made by me, hand painted with a brush❤️</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79id27q79sjc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1avnmnx</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>My peachy nail design.</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avnmnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1avn50i</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>2 hours work</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avn50i</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1avhr09</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Hearts of purple spring</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avhr09</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1avci6x</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Improving on nail art?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1avci6x</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb 22 08:07:55 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_25.xlsx
+++ b/data/2024_02_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C598"/>
+  <dimension ref="A1:C733"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10599,6 +10599,2301 @@
         </is>
       </c>
     </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ax0efu</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Emo Pop Art🕸️♥️</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ajgvbke783kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1awzkw2</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Do I have potential?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/anoxg5j8z2kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1awzal4</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Is Cirque Colors a good brand?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awzal4/is_cirque_colors_a_good_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1awynj4</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Question: Would gel nail tips cure well after I've done nail art on them?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awynj4/question_would_gel_nail_tips_cure_well_after_ive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1awyl1o</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Pretty proud of my second try with builder gel</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rwesqk5so2kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1awx2d9</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Finally kicked the habit!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awx2d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1awvvbu</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Picking at my nails</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awvvbu/picking_at_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1awv1wc</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Occasionally, I (inadvertently) match my nails to something I own 😄</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awv1wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1awwvz1</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi all nail techs! What exactly do you need to do to become one? </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awwvz1/hi_all_nail_techs_what_exactly_do_you_need_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1awwm70</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Loving these chunky glitter nails!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awwm70</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1awvx3t</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>how to stop biting nails?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awvx3t/how_to_stop_biting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1awvgun</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Pretty in pink!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxn4uxk7w1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1awuz2t</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Gel X Tips for XL Thumbs</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awuz2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1awuo97</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Set 😇 </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87w8zozip1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1awunz3</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wvty0ugp1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1awmsc8</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>went with some mets colors since spring training starts this week! 🔷🔶⚾️</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awmsc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1awtl6l</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Vacations Nails!</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hznzwl1mg1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1awtf83</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Haven’t had mine done in a while, I’m happy 😊</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s195prc8f1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1awsyd8</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Ready for Springtime</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czahtseeb1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1awsk28</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Nail growth journey 😀💅</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awsk28</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1awsgef</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Round and almond are not created equal </t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4rlsy3j71kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1awrmw7</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>My first time doing gel with no tips</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awrmw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1awrcuj</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>I tried semi cured gel nail strips and so far I’m so happy 🥰</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awrcuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1awqqp7</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Sparkling in the sun</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awqqp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1awqdhd</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Took me 2 hours but it was worth it </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qf9par5s0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1awq9ln</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>I have 2 questions whenever I grow out my nails sometimes there would be a piece of top layer of my nail that will come off or looks hallow and I would take it off, How would I avoid this and what causes it?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awq9ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1awptlb</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Haku nails from Spirited Away 🤍🐉</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivagi1n8o0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1awplu0</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Hey I recently started growing out my nails and..</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awplu0/hey_i_recently_started_growing_out_my_nails_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1awpjeb</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>🧡 Painted Polish Gourd Vibes Only 💛 Who says Halloween shades can't double as Spring shades? 😆</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awpjeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1awphar</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Clowning around 🤡✨</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1td1m9nql0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1awpfm9</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>So I painted my nails periwinkle and then added a cat eye on top, what do we think ?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awpfm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1awp7yn</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>liquid gold</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx4zrtgwj0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1awodnx</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Dip or acrylic?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awodnx/dip_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1awo98i</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>The Chrome was just not chroming for me on today’s set. But the opal is definitely opaling.</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awo98i</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1awnfsm</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Back to the basic…..</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awnfsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1awn9ri</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Natural nude look</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awn9ri</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1awmko8</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Love these spring nails!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r31uglmd10kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1awmc4p</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Icey Blue</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwkioskmzzjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1awlwb8</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Yippee!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awlwb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1awlqh7</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where to start with mani/pedicures? </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awlqh7/where_to_start_with_manipedicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1awllbj</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>First set of Gel X nails done by me, on me ❤️</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awllbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1awkyy7</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>blue chrome 💙</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvwwwly0qzjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1awkg1f</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Subtle skies ☁️</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6sekvhemzjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1awjqdw</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>First poly gel attempt !</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awjqdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1awjkvw</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>beautiful long nails</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpcjocx8gzjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1awiatk</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First day. Would it be ok to go back and ask to clean up my cuticles? </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7ux15cc7zjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1awhso7</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>How to keep soft gel nail tip cured with soft builder gel from popping off so soon?!</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awhso7/how_to_keep_soft_gel_nail_tip_cured_with_soft/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1awhff4</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Lacquer nails not covering the tip - need advice.</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awhff4</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1awgwql</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>where do you guys get your glue on nails?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awgwql/where_do_you_guys_get_your_glue_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1awgsr0</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Dual forms and builder gel</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1awgsr0/dual_forms_and_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1awgsef</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Copied a design</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajvl1vcuwyjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1awf3e1</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Nails match my weights</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awf3e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1awgmdr</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4l78ji1nvyjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1awg9m0</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Tried forms for the first time - advice needed!</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqzplrp4tyjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1awf3xp</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Retro</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v5nmyqzkyjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1awezc0</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>These were so fun and frustrating to do!</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awezc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1awex1h</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Check out this cuticle progress! Really proud of myself...</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awex1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1awelfu</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Not as fresh anymore, but its my first red acryl. ❤️🌹</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awelfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1aweinp</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>What do you think of my nails? Be hard if you want, I need honest opinions</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpgxadzpgyjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1awdmto</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>New set done yesterday!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5j6iov9ayjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1awdljn</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Pink french ❤️</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x16gvjy9yjc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1awddmq</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Which is better for my hands?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awddmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1awd6th</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Milky White Nails</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ir2a02ct6yjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1awcyq8</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favourite color totally white </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7r2zaq15yjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1awbcsf</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Shape ok?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8t806kbrxjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1awazbr</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Tried something different and fun!!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwwwfegtnxjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1awa5eb</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with this Pink design 💖 </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aor74yggfxjc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1aw9zip</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Holiday ready! Pastel French tips and flowers on acrylics</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i0fy67smdxjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1aw5dww</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel polish without acrylates </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aw5dww/gel_polish_without_acrylates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ax08mm</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>im amazed by this combo</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax08mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1awzz3v</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Gotta favor...need a linerar, blood red holo, blue based, no orange</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1awzz3v/gotta_favorneed_a_linerar_blood_red_holo_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1awzw3s</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Almost the perfect nude?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oggh1qah23kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1awxc8e</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>I finally got my Lurid Lacquer order!!!</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awxc8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1awvo7c</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Like purple Terrazzo tiles...</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpsu7o6zx1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1awt8hn</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>A lighter color for a change from my dark autumn/winter faze lol</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfwj8crpd1kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1awsqan</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>I love it, but is this a turn off?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awsqan</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1awsf2u</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>The many faces of Dudley nudshite 😂✌🏻</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awsf2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1awrpow</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>ILNP: No Promises (metallic/holo)</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nj9drzy021kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1awqx5w</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>A classic dark crème palette cleanser before spring comes!</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrvlq083w0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1awqv8q</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>This weeks mani</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awqv8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1awqmqw</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>My new favorite 👽🛸</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awqmqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1awqjvf</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>I’m ready for spring 🥰🍓🌸</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awqjvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1awq7he</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Organize by color or brand?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3g57jszq0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1awq7go</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>ILNP MEGA</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awq7go</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1awq5bh</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>hehe</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xelllcjq0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1awq4dg</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Reminds me a Lily pads</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awq4dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1awpokv</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Loving this look!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awpokv</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1awpib5</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Neutral Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awpib5</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1awpi2b</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>🧡 Painted Polish Gourd Vibes Only 💛 Who says Halloween shades can't double as Spring shades? 😆</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awpi2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1awp37m</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Revlon Electric 🩷</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awp37m</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1awp0zx</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Ready for Spring!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awp0zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1awom6t</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Larkspur-Cadillacquer 💙🪻💖</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7aulklwf0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1awo5gx</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Loving the pink shift on this olive green!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2cnhggnc0kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1awnkxe</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>ready for spring training! ⚾️🔷🔶</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awnkxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1awnhw7</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Aquamarine by People of Color Nail Polish</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybw9qyqy70kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1awmy7q</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Trying the vertical cat eye to velvet method!</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p8gidi8340kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1awmknz</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Mooncat Merkitten</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awmknz</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1awlx8h</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Felt a bit green</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9chwceowzjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1awlucz</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Mooncat and Ube Jelly Skittle</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awlucz</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1awl8ha</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Getting Ethereal Lacquer in Canada??</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1awl8ha/getting_ethereal_lacquer_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1awkfoy</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Helpful lazy tip</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1awkfoy/helpful_lazy_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1awk6l2</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Make it Pink! Make it Blue! 🎀</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awk6l2</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1awk6kc</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>First Time Poster 💜</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awk6kc</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1awjmvn</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>I grew my nails for 4 months, got my first manicure ever, and 3 days later one of them broke. What should I do?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awjmvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1awj2k1</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Taupe jazzed up</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/bPn0P36</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1awioap</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My nail chipped off. Trying to decide on a shape, please help!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awioap</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1awfhh4</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Nice starter kit?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1awfhh4/nice_starter_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1awf6sj</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Self conscious about deformed thumbnail. Solutions?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awf6sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1awd4l1</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Cath Kidston inspired nails 🤍🌹</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awd4l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1awglph</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>ILNP Black Magic in different lighting</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awglph</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1awfuqa</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>In love with this combo :)</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4t7tug8qyjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1awfij3</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Ethereal Howl's Moving Castle</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1awfij3/ethereal_howls_moving_castle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1awehnw</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>First Mooncat polish and I am hooked</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awehnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1awehg1</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>What’s helpful in a review ?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1awehg1/whats_helpful_in_a_review/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1awe7lk</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>🧡⚡️Ziggy Stardust⚡️💙</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awe7lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1awdn5q</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Was disappointed in my velvet nails attempt until I saw them under my bedside lamp the next morning</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awdn5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1awdky6</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Snake Charmer 🐍</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awdky6</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1awd5du</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Simple New Year's manicure</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxc2q83i6yjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1awclfq</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>sparkles in the sunlight ✨</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awclfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1awalty</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>What would y’all do?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awalty</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1avvivf</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Need help</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1avvivf/need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1aw3kfo</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>cnd shellac shades discontinued</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aw3kfo/cnd_shellac_shades_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1awz9lp</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monochromatic </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pfn1yuxv2kc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1awrx96</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>I am the nail tech and these are my first two cartoon designs, looking forward to keep practicing this type of designs ✨🥰</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctsvboci31kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1awocn9</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>The chrome isn’t chroming today, but the opal is definitely opaling.</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awocn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1awn9zf</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I am the nail tech and this was done on myself</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awn9zf</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1awm9z7</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pop Art &amp; Emo Inspired </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01n0zpb6zzjc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1awkndk</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Thanks to my amazing nail artist Nazza I was able to make these inspired favorite anime nails a reality</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvehbqeumzjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1awjely</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Ombre Pink</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1awjely/ombre_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1awi9d1</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>First posting &amp; first time trying 3D art as well 😊✨</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zyr111r27zjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1awh30v</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Y2K mix and match nail art 💗✨</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awh30v</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1awfwkd</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Cath Kidston inspired nails 🤍🌹</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1awfwkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1aweg03</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Simple set with nail art made by me. Hope you like it 🖤</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3evln98gyjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1awc61b</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slytherin Nails </t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh2m466lyxjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1awc4tw</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Slytherin Nails</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnfbcveayxjc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb 23 08:08:22 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_25.xlsx
+++ b/data/2024_02_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C733"/>
+  <dimension ref="A1:C861"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12894,6 +12894,2182 @@
         </is>
       </c>
     </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1axum88</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>What’s everyone’s favourite nude shades at the moment?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axum88/whats_everyones_favourite_nude_shades_at_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1axtv4k</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>nailbed recovery?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axtv4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1axqej8</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Can I use colored builder gel to apply clear tips to natural nail?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axqej8/can_i_use_colored_builder_gel_to_apply_clear_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1axu0yo</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>What grit file to prepare nails for normal polish?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axu0yo/what_grit_file_to_prepare_nails_for_normal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1axkx9u</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Infill Bio Sculpture with Bio Gel</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axkx9u/infill_bio_sculpture_with_bio_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1axt5tn</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>recent 🤭</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7su9yna7y9kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1axt1v0</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Can I just show off my natural nails for a minute? 🥹</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axt1v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1axsvew</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Short Almonds - a mistake?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axsvew</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1axs5ka</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Can you do almond shape now?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tzbolo7o9kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1axqxpu</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>I don't know if I should get a coffin or stiletto nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdzg7fwec9kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1axquj1</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>something simple but the dopamine still hits 🥹</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lb4b2kkb9kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1axql4n</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>It's giving chiclets</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hyp5i8799kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1axqgy7</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Shego Nails 💚🖤</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psif63o589kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1axqeav</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>How my Cirque mystery bag came</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axqeav</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1axp4it</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Acrylic nails</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axp4it/acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1axp205</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Made a set of green marble press on nails</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eihrkudsv8kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1axou58</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Press on nails pricing help?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axou58</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1axojpb</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>i love chunky nails :) on me by me</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icqmb8mfr8kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1axnsy4</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I drafted an entire post and lost it all 😭</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axnsy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1axnis2</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Best magnetic cat eye gel</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axnis2/best_magnetic_cat_eye_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1axndsu</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Sticky tabs for press-ons!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mhl73nih8kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1axmi0y</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Birthday nails!!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bykzui1ja8kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1axmhm3</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Simple but I adore them 💓 🎀</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztebyufea8kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1axlyhf</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Best nail designs for fast-growing nails?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axlyhf/best_nail_designs_for_fastgrowing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1axl4h7</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Kept it simple this time 🍀</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wquqx2s508kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1axiys7</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Why does my ombre have texture?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pstf1vlqk7kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1axdv9x</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>What to do about this bulge on my side wall?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3voz9czxk6kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1axk3z6</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Went with cat eyes today</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcw41lxws7kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1axjoug</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>First time going ‘bare’.</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8hz874yp7kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1axiu0e</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My nail tech relocated</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axiu0e/my_nail_tech_relocated/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1axiqax</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Era's tour nails 💅✨</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4syuz8l0j7kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1aximd4</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to stop edges lifting when using UV cure </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aximd4/how_to_stop_edges_lifting_when_using_uv_cure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1axigfu</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Chrome peeling off</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9mtly73h7kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1axdblm</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to decide on my next pedicure color </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axdblm/trying_to_decide_on_my_next_pedicure_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1axdygz</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>New set😊</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8u8piswjl6kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1axhbau</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I usually do nail art on every nail so this feels plain to me😭 any ideas appreciated</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7os2bf6197kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1axgz90</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>showing off my new nails @ school 🥰🎀</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axgz90</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1axgx1y</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails perfect for spring </t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktw4jl4567kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1axaxmq</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help figuring out what was done to my nails? </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axaxmq/need_help_figuring_out_what_was_done_to_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1ax1r2t</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Sally Hansen Insta Dri Product List?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ax1r2t/sally_hansen_insta_dri_product_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1axgonk</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Milky 🤍☁️🐚</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ho8dc66m47kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1axgc5j</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Selfmade</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axgc5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1axgb5r</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Cheshire Cat 🔮 ✨</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axgb5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1axfph3</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Playing Around</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdszu2j1y6kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1axfgf1</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Who else loves short nails? ₍ᐢ. .ᐢ₎♡ ༘🌸</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axfgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1axf93z</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>What color should I paint my nails for an interview?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axf93z/what_color_should_i_paint_my_nails_for_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1axexjr</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>🍃💚 earthy groovy mani</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibnlntfhs6kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1axed22</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>What to do with grow out?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axed22</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1axe9iq</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gorgeous cat eye done by my awesome nail tech. </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hyno7oign6kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1axdoyp</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>I call them my space mermaid nails! 🧜‍♀️🐠🐚</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axdoyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1axd9il</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Just back from the nail salon</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvuqoaktg6kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1axcy02</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Longer Nails - Hard Gel vs Soft Gel</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axcy02/longer_nails_hard_gel_vs_soft_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1axcve6</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Zoinks Scoob!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axcve6</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1axc30i</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>I haven’t done a sponge ombre in a while.</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g06wts7m86kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1axbdl6</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Matte black &amp; flowers inspired by textile print</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axbdl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1axbdcy</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Opinion?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axbdcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1axb6fp</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Update for everyone who wanted to see the nails with the ring!</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cy1lmrh26kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1axb5bs</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Star Wars BIAB Nails</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axb5bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1axaiy4</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>I asked for something space/galaxy-ish. ✨</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zn6eaunwx5kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1ax9s4f</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>First time doing semipermanent at home. What do you think?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax9s4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1ax9l1j</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Been a rough week for the girls. In need of a good strengthener. What are your recommendations?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpd71ji9r5kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1ax9jig</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>I can’t keep my nails any longer than this because they bend and break. What should I do?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax9jig</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1ax9hgg</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honestly love builder gel so much! </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mvhfk6jq5kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1ax9d6g</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Is almond my shape?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax9d6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1ax98ex</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Just got these adorable fruit designs from an artist in Japan</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax98ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1ax97bs</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Cow print nails</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax97bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1ax8kb3</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>💕</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvjl8ppmj5kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1ax89fz</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Buying OPI gelcolors and Biab products in Europe</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ax89fz/buying_opi_gelcolors_and_biab_products_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1ax6zf9</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Should I be the one to pay?!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ax6zf9/should_i_be_the_one_to_pay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1ax6ro5</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Tips?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax6ro5</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1ax62vt</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Can I use peel off base coat over acrylic?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ax62vt/can_i_use_peel_off_base_coat_over_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1ax4nsj</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Not typically a red gal, but I think I like the negative space + red combo! Photo from my salon's IG.</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wi5jw243l4kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1ax1t39</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Question regarding DIY press-ons</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax1t39</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1axv8u4</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Help me match this colour! (Please)</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44djgs2jlakc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1axv4pt</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Rubber base won’t adhere to tip of my nail</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axv4pt/rubber_base_wont_adhere_to_tip_of_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1axu7p1</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>What are your favorite "ugly" polishes?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmp5clze9akc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1axsuad</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticle oil alternatives? </t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axsuad/cuticle_oil_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1axrn8i</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunspin by avon </t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gl0xxv87j9kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1axrfdb</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Currently mourning the sudden, tragic, and unexpected breaking of my middle nail 😢</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k07wpdw2h9kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1axqx2x</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Looking for cracking nail polish</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axqx2x/looking_for_cracking_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1axqv5e</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>I can't stop staring at my nails</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axqv5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1axqiy4</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Newbie Inspired by Winter</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axqiy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1axpscl</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">manucurist brand question </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axpscl/manucurist_brand_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1axq0ec</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Loving 💚 Greens about to change it to another</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axq0ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1axq0c3</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>My Valentine's nails &amp; first attempt at nail art ♥️</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axq0c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1axpsq5</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Mooncat - Garden of Evil</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axpsq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1axpe8q</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Aeromancy</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axpe8q/aeromancy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1axojgp</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Beaux Reves - Fawning Over You (as topper)</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b3yzz39br8kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1axo3zc</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>As a blue lover, do I need House of Hades???</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axo3zc/as_a_blue_lover_do_i_need_house_of_hades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1axo1bn</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Two Questions</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axo1bn/two_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1axnvzz</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>I’m just too excited for spring!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2u5w70ql8kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1axnllr</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Magnet</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axnllr/magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1axn2bt</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Thermal and flash reactive?!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axn2bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1axmy6j</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>first post but here’s my polish</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axmy6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1axmica</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Celestial vibes</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axmica</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1axiwye</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Holo Taco Curfew Crasher</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axiwye</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1axjjyo</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Love this color! 🍩</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rd4lvtzo7kc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1axj7rg</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Phoenix - Louis</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axj7rg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1axiusv</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Comet ☄️</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axiusv</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1axiil2</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>i finally got my hands on my dream polish</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axiil2</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1axgz4d</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>ILNP “Staying In” out and about</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axgz4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1axgmsn</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>The horseshoe magnet lives up to the hype 🧲</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j9s1of3947kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1axg4ie</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>ILNP Spring Launch</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axg4ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1axg3ye</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Cheshire Cat 🔮 ✨</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axg3ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1axg2jk</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>I’m just over here making magic</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/keooxf2i07kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1axeb4p</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead since it’s not Friday yet</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axeb4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1axd5e5</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Been feeling like Dam Dingle Berries 💩</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axd5e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1axcd8d</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Mooncat - To All Who Ghosted Me</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axcd8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1axbqgk</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Help me describe this purple!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr919sg466kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1axb05d</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Favorite purples? Pic for attention</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47oe5ku916kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1axa8mk</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Drip dry drops</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axa8mk/drip_dry_drops/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1axa7kv</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Hershey Kiss collection</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axa7kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1axa36m</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>HALP!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axa36m/halp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1ax9gaz</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>MSM - The Day I Tried To Live</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/35mne0p6q5kc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1ax9d3u</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Color Club no longer shipping to Canada?!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ax9d3u/color_club_no_longer_shipping_to_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1ax8v60</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Green nails are quickly becoming my go-to 🫒</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwwmcfqwl5kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1ax6zcy</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>✨sparkly skies✨</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax6zcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ax4asm</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Favorite toppers?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ax4asm/favorite_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1ax1aok</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Dreamscape</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax1aok</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1ax1790</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>What brand is this?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax1790</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1axv5qe</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Press On Nails &amp; Price?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axv5qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1axuk0d</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to get better at nail art! Any tips are welcome!  </t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hen40rcadakc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1axr5nh</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>HAZBIN Hotel nail art</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oehaksfie9kc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1axr2c9</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>My first spring nail design</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ew3g7w0jd9kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1axkitr</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Casual purple nails</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axkitr</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1axhatr</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axhatr</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1ax5m1f</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Fancied something different ✨</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ax5m1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1ax5hxv</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfboiuawt4kc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb 24 08:06:49 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_25.xlsx
+++ b/data/2024_02_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C861"/>
+  <dimension ref="A1:C994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15070,6 +15070,2267 @@
         </is>
       </c>
     </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ayonlc</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Nails🤍🤍🤍</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqkqkvd9jhkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1aynf86</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>French with Neon green tip!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aynf86</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1aym995</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>loving the opposites!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aym995</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1aykt2w</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>These two birds come to our nail salon everyday, and these specific ones always try to get in. Why?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vr5oojynggkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1ayk5v8</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Almond or Square? Which looks best?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8eulrrsagkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1ayjwms</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Granddaughters first design</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjmei1vh8gkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ayjsq9</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing glittery gel...love the sparkle </t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcmlcn0k7gkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ayispl</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>It’s A Sad Day…</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7u6mrptvyfkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ayihxu</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>my nail tech ATEEEEE!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayihxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ayides</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>New nail tech</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayides</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1ayi2zu</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Enchanted polish</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayi2zu</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ayhyhr</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Golden Hour</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8za3xfmprfkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1ayhwle</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Look my new set 🩷💝💅</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1z39hy7rfkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ayhn59</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>How to use??</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayhn59</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1aygzld</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>sorry nail bed</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aygzld</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1aygzi3</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tz57q7pjfkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ayglnz</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Haven’t had my natural length this short in a while! (After/Before)</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayglnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1aygh6v</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>My first set, hopefully not last</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aygh6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1aygglb</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I love my nail tech</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uggotfkffkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1ayg7ui</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Homemade gel nails</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayg7ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ayftrx</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>New nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayftrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1ayfpqm</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>what do we think?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8p7vhp8y9fkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ayfhrx</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question for those who regularly wear long (glamour length) nails. . . </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ayfhrx/question_for_those_who_regularly_wear_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1ayceec</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Growing my nails out for the first time</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayceec</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1aycce6</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Durable press ons?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aycce6/durable_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1aycaw5</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I did these for a friend... I get bored and learn new skills and she gives me Pinterest inspo ☺️🙏🏼 (her natural nails)</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scwwjeqxkekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ayey6n</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>What do we think of the apex on these? Too big?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayey6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ayeup8</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>It's simple but idk I just love this colour</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et8htudi3fkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ayej06</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>How to remove this black stain on my UV Gel?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayej06</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1aye90w</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Help! Get dark hair dye out of gel nails?!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aye90w/help_get_dark_hair_dye_out_of_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1aydqu9</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>First attempt at gel nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztk2j8divekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1aydm5g</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>First time doing gel extensions!</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aydm5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1aydf0a</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>valentines</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aydf0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1aycy3a</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Absolutely loving these press ons</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prz2b75ppekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ayclui</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Cow print nails 💅</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7eoayca6nekc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ayby6h</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>All Too Well by Pahlish🧣</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7h9jrkeiekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ayb6zg</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw0w7fyycekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ayat4x</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Second time using rubber base</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayat4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1aya8z0</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>baby blue french gel x done at home (:</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aya8z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ay9p07</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Thoughts on my nail shape?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkpw66062ekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ay9cef</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>No UV gel strips?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ay9cef/no_uv_gel_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ay9azh</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Learning how to do my nails as I grow them!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay9azh</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ay8zjq</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Blueberry nails 🫐🫐</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lvh7vszwdkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ay8xye</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Sparkly french doticure!</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1smkzqsjwdkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ay8f9r</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>First couple of times using a at home dipping kit</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay8f9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ay804g</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Young nails monomer !</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ay804g/young_nails_monomer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ay7w23</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>I did regular white french last time, now i did more of a gemmed up pink frenchy, thoughts?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay7w23</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ay7tpw</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>natural nails ❤️</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay7tpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ay7kiu</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>✨🌿</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by7bl4bvmdkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ay7k1v</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Cuticle care with fake nails</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ay7k1v/cuticle_care_with_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ay7bmi</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>How do you feel about these nails?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay7bmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ay7766</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Pink Unicorn Mani</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay7766</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ay7avq</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>🙂🙃</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j8ozr6zkdkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ay7acb</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>obsessed with my new nails</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay7acb</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ay6dqv</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Hey nail girlies, question, are there fake nails that you can take off and wear again later for a long time? Like re-usable nails? What makes them different from the regular ones?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ay6dqv/hey_nail_girlies_question_are_there_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ay63yb</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Do these nails look good?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay63yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ay5wqi</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Manicure ( gel )</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5gzmoyhbdkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ay5qw2</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Lunar New Year nails</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay5qw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ay3dw3</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Some of my nail art</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay3dw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1axwmie</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was super gluing something and it accidentally got on my acrylics. How to remove without damaging them? </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1axwmie/i_was_super_gluing_something_and_it_accidentally/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ay4mrn</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>nail growth update :)</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay4mrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ay3wf4</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Fun ways to color acrylic??</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ay3wf4/fun_ways_to_color_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ay3qcd</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Simple ❤️</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zoru7507wckc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ay3eo2</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Coolest nails I've ever had :)</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay3eo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ay32dw</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>What do you think of this design?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2ldcwvdrckc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ay1ob4</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Do my nails look weird or cute?!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay1ob4</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1axzxcg</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Nude!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1p63fzj2ckc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1axzsjv</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Got this for less than 20 usd in the ph! (nail art + builder gel)</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2up9noc1ckc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1axyh2z</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Kiss Salon Acrylic French Nude</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axyh2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1axxr18</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Happy Friday 🩷</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94wfkypdgbkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1axx4wc</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Flaunting the Tortoise</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axx4wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1axvawc</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Floral sticker set</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1axvawc</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1aynnkt</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Nail wraps and nail polish allergies?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aynnkt/nail_wraps_and_nail_polish_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1aymc0y</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Got ghosted but at least I have cute nails</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a04qbij4vgkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1aylhj9</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>So nice I bought it twice… 🫠</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc956971ngkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ayklfi</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Frosted Metals are so underrated</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayklfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ayhfi8</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>My first bath milk attempt! Inspired by this sub.</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufjnq1y9nfkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ayherk</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Artemis Deathkiss Space Mani</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayherk</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ayhcx7</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Obsessed with this combo - my nails are glowing 😍 + dog photo at the end</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayhcx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ayh8bx</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Weird marks on my nails after removing dip powder</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayh8bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ayeool</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Best skittle I've ever done 💅</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayeool</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ayeolj</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Blessed with Beauty and Rage 💐🔪</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayeolj</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ay7hzu</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticula Mic Drop replacement </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ay7hzu/cuticula_mic_drop_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1aydivv</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let's talk about cuticle removers </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aydivv/lets_talk_about_cuticle_removers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1aydk88</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Recovering from a nail break and trying square nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aydk88</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1aydadm</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favourite Glow in the Dark? </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aydadm/favourite_glow_in_the_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ayd8bj</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>I'm speechless</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/29436cwqrekc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ayc2ez</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Enchanted Polish</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayc2ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1aybxp2</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>All Too Well by Pahlish🧣</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0oe6hm4biekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1aybo4a</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Love me a mag [Polish] - ILNP Jet Setter</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aiyv97d3gekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1ayb3ur</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Impossible-to-dupe shades?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ayb3ur/impossibletodupe_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ayabxh</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Lens Flare!!!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayabxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1aya84a</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Glasswing Butterfly (PPU Feb 2024) is really lovely</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aya84a</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1aya1he</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Nailed it 💅 (what I got and what I sent as inspo)</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aya1he</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ay9wg5</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Going Salon Free / Healthy Nails</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/km5ofyco3ekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ay9chj</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>I am the moment... Wow!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9kglq4hzdkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ay8zsd</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Full moon(cat) manicure 🥵</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay8zsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ay8hgp</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>I will never get tired of this shift</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hn8kftzatdkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ay8gvu</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Moving... maybe a lot - how to do this?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ay8gvu/moving_maybe_a_lot_how_to_do_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ay87xy</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Not a horrible first attempt</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6h6h3serdkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ay81gs</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Brands and products to gift young ladies</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ay81gs/brands_and_products_to_gift_young_ladies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ay7uk6</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Went and got my nails done and It's Giving magical girl/Sailor Moon and I love it</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wums1zpsodkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ay7f8c</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Rainy day glow</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzaph2buldkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ay7bvl</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Warm winter 🌻</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wswk3s6ldkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ay78l0</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>It’s a palette cleanser to me!!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e51xlxtikdkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ay6y4v</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Mooncat- Queen of the dead</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay6y4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ay6lxm</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Improving so much since I joined this sub!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay6lxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ay5k1i</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Phoenix Lacquer vs Ethereal Lacquer, can you tell me your experiences with bottle sizes and quality?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ay5k1i/phoenix_lacquer_vs_ethereal_lacquer_can_you_tell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ay583p</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Canada No Smudge/Water-Based Top Coat Reccs?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ay583p/canada_no_smudgewaterbased_top_coat_reccs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ay4mjf</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>My first go at crackle polish!</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47jjfy1i2dkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1axxyyx</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Base Coat</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axxyyx/base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ay4bbg</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Bluey nails- for real life!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay4bbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ay41yq</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Louis- *in throes of increasing wonder*</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay41yq</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ay3nkc</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>🌈 Yellow Rainbow Shatter 🌼</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay3nkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ay2ix1</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Attempted a chrome look without gel!!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay2ix1</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ay2d6c</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Mooncat - Garden of Evil</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay2d6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ay1zlr</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Naruto nails!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm4tkrkkjckc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1ay1sye</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Comparison Swatch - Mooncat Velvet Rose with Matte?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdg5pn47ickc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1ay1q50</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Lavender glow ✨</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay1q50</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ay1ipt</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>opinions abt sensationail gel polishes?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ay1ipt/opinions_abt_sensationail_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ay167n</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Colors - Mood Ring (velvet) </t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3otxwh0adckc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1axx1kv</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Nail Care for swimmers</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1axx1kv/nail_care_for_swimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1axx0l8</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Need recommendations for a metallic shine green nail polish that looks like the one this streamer is using. OPI is the preferred brand, but is not a must.</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adhlfkie7bkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1aynde5</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Long Nails VS Short Nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzqaq0z65hkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1aykxmt</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Started doing nails</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnej8wjthgkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ayftk6</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>I decided to do some spring nails last night. Do you like my birbs?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayftk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ayfdrs</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Cat eye nail deco</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0370rxig7fkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ayfbzb</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>inspired by @jayseenails on insta</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9mvgw737fkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ayf0b7</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Hey, this time I switched to a simple but satisfying one!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30bbcfpn4fkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ayb2zc</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Today’s nails are sweet and flirtatious for my client🎀</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbil4r6acekc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ay9hdx</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Stonework</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay9hdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ay5sfg</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Emo nails</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay5sfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ay5s41</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Lunar New Year nails</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ay5s41</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb 25 08:06:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_25.xlsx
+++ b/data/2024_02_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C994"/>
+  <dimension ref="A1:C1163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17331,6 +17331,2879 @@
         </is>
       </c>
     </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1azici4</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>One of my favorite set that I did last year!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azici4</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1azhr8v</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Recommendations on products for damaged nails?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1azhr8v/recommendations_on_products_for_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1azh819</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Still learning</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azh819</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1azh47h</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>A healthy way to remove lacquer??</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1azh47h/a_healthy_way_to_remove_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1azgbzx</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Im so inlove with these nails!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gl8gqah5okc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1azg4b3</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Options for thin nails?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1azg4b3/options_for_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1azg0uk</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Lovin' it!</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mn4e35e2okc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1az9xpb</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Xenomorph Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az9xpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1azfc2y</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first press on nails! </t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzsii2apvnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1azdddz</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>What is this indent in my skin caused by my nails called? And how can I get rid of them?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azdddz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1azcepw</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>What would cause chipping this soon, bad prep??</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azcepw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1azc872</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>I used gel sealant on my press-ons how do I get them off?😭</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/600dalst2nkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1azb5nu</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Are badly done acrylic nails fixable?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1azb5nu/are_badly_done_acrylic_nails_fixable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1azf4j1</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>So clean, love it!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxxje0rgtnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1azf36i</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Is this the proximal nail fold?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2itiwur8tnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1azew5f</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Engagement nail into help</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1azew5f/engagement_nail_into_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1azes7e</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help please—looking for advice </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1azes7e/help_pleaselooking_for_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1azdvem</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>tried something new!!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azdvem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1azdlkp</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>All things glitter 😁</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv43rmf3fnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1azdjmq</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Feeling clowny!</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azdjmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1azdd3a</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>A simple but pretty pear-shell nails 🐚🧜🏻‍♀️🎀🥰</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azdd3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1azd9pk</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Nail growth with Acrylics</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1azd9pk/nail_growth_with_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1azcygt</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>new set! trying to figure out which shape works for me 🥰</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azcygt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1azcwwq</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Which shape for my hands?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azcwwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1azayy8</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>I’m obsessed with purple 💜</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kscn10t7smkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1aza3yf</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Black flowers and french tips</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ei7se7s7lmkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1az9yp4</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>what do yall think? tried a new style, worth $60?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az9yp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1az9j9y</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>What to do with long natural nails</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1az9j9y/what_to_do_with_long_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1az8ulh</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Simple pastel flowers 💐</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m6lpixhbmkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1az8iqp</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>My birthday/ camping nails. #piscesseason</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az8iqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1az60ap</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>How do you get the last 1/4 of polish out of the bottle?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1az60ap/how_do_you_get_the_last_14_of_polish_out_of_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1az7og7</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>My favorite go to 🩷🤍</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45uwgs6o2mkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1az7goj</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Just got my acrylics removed and BIAB applied for the first time. Love it 💅💜</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w925ez711mkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1az7g4l</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Flowers!!</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvhs7pnx0mkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1az7eww</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Sometimes I like to do a secret design underneath!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az7eww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1az7ej3</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Obsessed with my new holographic nails!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vdg3mke0mkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1az765v</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Idk how I ended up with square again but I’m kinda feelin it</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnrlzj3vylkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1az6ew7</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>New nails, done by me</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3swmo7ctlkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1az5wt5</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>First time with this</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gtb63skplkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1az5vf7</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Current nails</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t9ry5lbplkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1az5isy</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>First Time Gel X Manicure</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az5isy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1az5hya</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Essie Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1az5hya/essie_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1az0mof</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Adven-spore awaits!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxb2uryvmkkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1az0edo</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Why do my magnetized nails always change</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7waewr9lkkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1az4tqj</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Spring nails💐🌸🩷💓</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az4tqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1az4qd0</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>How to make press ons look natural</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8i3kja4hlkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1az4ekc</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>90s nostalgia nails 💿</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gk0dclspelkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1az3y9k</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>st. patty’s day nails 💚</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az3y9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1az3wvu</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Usually get my nails done at the salon but I’m low on cash so…</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uiiokao2blkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1az3rct</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>I must be doing something wrong but idk what it is....</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1az3rct/i_must_be_doing_something_wrong_but_idk_what_it_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1az3p9k</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>DIY GEL NAILS</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az3p9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1az3jb5</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Tried something different this time</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgza4uv88lkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1az371g</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>My nails today</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxu4zu1m5lkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1az2n1f</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i feel magical </t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6nbqqedh1lkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1az1toi</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Something a bit brighter than I normally go for but I love them</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwrhefjnvkkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1az1j1y</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Current Nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rplmc6ihtkkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1az154l</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>My left hand is black French tip and the right is white.</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az154l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1az11lb</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>At home BIAB with gel polish nail art</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qgll4expkkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1az10b9</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>I got my nails done today, with a matching pink case that i'll never use again</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfhi966cpkkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1az0e7f</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you mix polygel and gel Polish? </t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1az0e7f/can_you_mix_polygel_and_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1az04te</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Color Club’s Ocean Spray over black 🤩</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c389i0sbjkkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ayyvdy</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>First time trying PolyGel</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax3xrs37akkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ayxhh1</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>I asked for "nude", I think she heard "clear"</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayxhh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ayxr6h</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Thought I'd treat myself while in Town</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh7gpjqu1kkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ayxmg1</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Trying out gel polish with a matte top coat.</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayxmg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ayxc5y</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icz1ve9uyjkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1aywt2t</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>♥️😍♥️</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aywt2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1aywha0</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Got some cute new spring Easter nails! I feel like a kid again. 🎀🌼🧡🍒🌸🐰🌈</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/055jz61asjkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ayw6ri</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out BIAB nails for the first time </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w09e3rvpjkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ayvwof</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Dip powder nails question</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ayvwof/dip_powder_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ayv7hr</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Love this colour!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvx8a0uyhjkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ayuub0</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Dragon nails!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayuub0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ayumxa</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Black and Chrome ombré aliens. 👽</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1utogbi0djkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ays77z</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>French manicure with the stickers?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ays77z/french_manicure_with_the_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ayuh7s</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Some nails I’ve done this month!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayuh7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ayho31</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Professional acrylics to prevent nail biting</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ayho31/professional_acrylics_to_prevent_nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ayh7r8</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>SALVADOR DALI inspired nail</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayh7r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ayu7eb</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Spring flowers</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayu7eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ayeap2</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">advice needed - so frustrated with gel nails </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ayeap2/advice_needed_so_frustrated_with_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1aytxj2</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Nail art as someone who can’t even draw a stick figure?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aytxj2/nail_art_as_someone_who_cant_even_draw_a_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1aytaun</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First time doing gel nails at home</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aytaun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ayszh4</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Homemade gel nails</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayszh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1aysv50</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>First time getting my nails done</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82yfjrn3wikc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1aysb52</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Marble nails with gold swirls ✨️</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aysb52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ayplkz</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>My 4th set ever!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mn0ywuy8uhkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1aypk8c</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Clean set 💅🏼🎀</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k9us8nsthkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1azgvpc</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fool’s Gold or Gold Flake Taco? </t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1azgvpc/fools_gold_or_gold_flake_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1azg6yh</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Distance to the Sun (Thermal)</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azg6yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1azet3e</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>I'm really digging my galaxy nails.....Excuse contorted hand gesture, was the only way to get public library lighting to cooperate and also I'm dumb and not good at this. Brand: Emily De Molly. Shade: It Must Have Been (Magnetic)</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s092qzeaqnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1azeah2</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Glitter vortex? Sparkle galaxy? Not sure what to call these but they're pretty!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cev5x3sllnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1azdpvt</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Color Club - Rock Solid</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6qntjx6gnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1azdpsz</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Musings on color preference. </t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1azdpsz/musings_on_color_preference/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1azdk11</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Gel lifting after 1 day!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azdk11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1azdhz0</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Literally the most stunning mani 😩</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azdhz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1azcuoo</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Reaching Skyward As You Root</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/15dmpn4a8nkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1azct0g</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Feeling Uninspired</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eho6uh9w7nkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1azcnni</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Another Lyn B win for me</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azcnni</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1azcj6c</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Death valley nails omg ❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqcdar0i5nkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1az72da</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Holo taco Tax Haven + Choco holo French tips</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltvqg023ylkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1azbmkk</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Funky Flaky Skittle</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azbmkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1azavot</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Dupe for M&amp;N Sylph?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxyhkayirmkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1azaukz</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>inadvertent match (nails look horrible ik)</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d04kq9s9rmkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1azakp8</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Midsummers dream is my new fave</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azakp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1azah1k</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Chanel - Atmosphere 629</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azah1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1aza5qo</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Gorgeous Electric Pink</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aza5qo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1az9kw3</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Has anyone used Nailsupplyinc?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az9kw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1az9hft</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>BK Buzz Bag?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1az9hft/bk_buzz_bag/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1az995f</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Dammit Janet!</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az995f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1az961o</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Another Ether Dragon post</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m7b98abwdmkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1az90zo</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>“Dream within a dream” weekly mani</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az90zo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1az90vv</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Spotted. Advice for applying toppers over completed manis?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az90vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1az80rw</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>KBShimmer mystery polish</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az80rw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1az71g6</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Tortoiseshell babyyyy 🐢</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az71g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1az6vh2</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Bees Knees That Went Well</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az6vh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1az6uyb</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still working on clean edges </t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5q9rixkwlkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1az65ck</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Got my nails filled in today and I feel so cute! opinions?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxnc6mfdrlkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1az5wzg</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Something fun for a bowling birthday party</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az5wzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1az5u6z</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Anyone tried Cici's Nails or Froni Nails? (Press ons)</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az5u6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1az5s4z</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>polish Pickup phoenix lullaby</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az5s4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1az58t7</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>The Matrix themed nails 💚</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az58t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1az48ok</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>That glowww though + sleepy bearded dragon at the end</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az48ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1az3fhs</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Long nails bend at the middle</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bhnipnf7lkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1az38j7</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Green Eyed Monster 👽</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az38j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1az31ni</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>My nails match the vibe of my new fragrance.</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69ncs2gi4lkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1az2vzv</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Velvetine</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xvprc7b3lkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1az2vgh</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>DRK Nails DIY Artisan Polish Lab from January 2024 PPU</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az2vgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1az2v0w</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Adina just hits the spot today</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jem5sih33lkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1az2q7l</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Petals for a Narcissist ft. the cat tax</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az2q7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1az2hya</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>I like it</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g56kp93h0lkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1az2gac</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>introverde goes outside</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az2gac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1az2cmk</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Chrome (?) nails!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az2cmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1az21q6</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>You can't sit with us.</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az21q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1az1ile</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Speaking about true to life swatch photos. Not once did I see the shift that was in photos. How? (product list and link to promo photos in comments)</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yb4viizuskkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1az0ohy</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>First post- I've Seen Betta Days</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oiu7nvv9nkkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1az0nxh</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Fawn-ing over you 💚🦌</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az0nxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1az02k0</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>My first time with flakes!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az02k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ayzldb</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Stunning thermal - “Never Found It” by Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn8censffkkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ayz97m</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>THAT SHIFT THO</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1imks9lzckkc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ayyrec</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Green Opal Stone</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayyrec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ayyo3d</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Camera Can’t Capture Its Beauty 💜🖤</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayyo3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ayyjkd</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>jelly nails to cope with having to cut them short 🪼</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cla6xzs7kkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ayy2g6</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Velvet magnet- which is best</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.etsy.com/listing/1630471315/mani-mag-set-of-5-with-magnets-your</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ayxp4s</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Garden of Evil 🌿✨️</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayxp4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ayxl2a</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>My sister said it looks like blue mushroom</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayxl2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ayx905</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Icy ❄️</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayx905</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ayx8c5</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Just excited about my new press ons!</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayx8c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ayx82u</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Contentment by garden path lacquer</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayx82u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ayvyyn</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Help?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ayvyyn/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ayvp1a</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Butterfly wings 🦋</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayvp1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ayukq1</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Looking for opinions please - natural nails for 4 years, should I get powder manicure before trip?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ayukq1/looking_for_opinions_please_natural_nails_for_4/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ayqcje</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Quartz and Kisses 💋</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayqcje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1azie7o</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Gummy inspired!</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1azie7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1azg70r</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>DIY Nails - A little bit of Spring! 🌷</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39bnjj974okc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1azf63l</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Did my sisters nails for the first time !!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdx8t5q1unkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1azdmc1</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Proud of myself</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s732cx0afnkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1azar1i</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>The last unicorn nails</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1shwdnufqmkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1az7bht</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Occasionally I do a little secret design underneath......</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az7bht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1az6awa</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Latest set</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az6awa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1az60st</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Jjk nails 👁️</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az60st</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1az4xof</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Kinda weird, but I was trying to make them look like mood rings</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puncahxcilkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1az4f5r</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>90s nostalgia nails 💿</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5ougd3uelkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1az1xof</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>At home Acrylics, critical comments welcomed</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1az1xof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ayzxs5</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Fun sets this week 🤗</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayzxs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ayz2vi</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Trying out something new</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayz2vi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1aywidn</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Got myself some cute new spring Easter nails! 🎀🧡🌈🐰🍒🌼</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w08fzllisjkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1aywejg</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Abstract Colorful Paint Splatter</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0uppjuvnrjkc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ayvxcp</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>I love my shiny brown nails with drawing details 💅🤎</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1vhceitnjkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ayvdlt</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love them 😍💅🏻 </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prb1qvicjjkc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ayrq1h</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Here’s my first 2 sets as a beginner any tips?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ayrq1h</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>